<commit_message>
portal and property list
</commit_message>
<xml_diff>
--- a/data/db/properties.xlsx
+++ b/data/db/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nburmeister\Documents\_Development\AssetManagementPortal\data\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B90BDD-A0D8-4D59-9D0B-1F813CB4FDEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0AD85B-F66D-4C7D-8BA2-E4F73A8308E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27360" yWindow="2730" windowWidth="21600" windowHeight="10905" xr2:uid="{65CCAB74-0CA2-4D5F-9FC7-1AACCFC26E43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{65CCAB74-0CA2-4D5F-9FC7-1AACCFC26E43}"/>
   </bookViews>
   <sheets>
     <sheet name="PropertyData" sheetId="1" r:id="rId1"/>
@@ -4144,9 +4144,6 @@
     <t>acquisition_date</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -4617,6 +4614,9 @@
   <si>
     <t>Associated Bank</t>
   </si>
+  <si>
+    <t>property_name</t>
+  </si>
 </sst>
 </file>
 
@@ -60075,49 +60075,49 @@
       <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P31" sqref="P31"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="33.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="18" customWidth="1"/>
     <col min="9" max="9" width="14" style="1" customWidth="1"/>
-    <col min="10" max="10" width="43.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="20.33203125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="20.33203125" style="12" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="27.5546875" style="10" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="35.88671875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="26.5546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="19.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.88671875" style="19" customWidth="1"/>
-    <col min="33" max="33" width="18.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="43.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14" max="15" width="20.28515625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="20.28515625" style="12" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="27.5703125" style="10" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="35.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="26.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="19.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.85546875" style="19" customWidth="1"/>
+    <col min="33" max="33" width="18.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>190</v>
       </c>
@@ -60125,10 +60125,10 @@
         <v>191</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>206</v>
+        <v>363</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>192</v>
@@ -60173,58 +60173,58 @@
         <v>205</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="V1" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="W1" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF1" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="AG1" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="AE1" s="19" t="s">
-        <v>322</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>323</v>
-      </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AH1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="AI1" s="19" t="s">
-        <v>306</v>
-      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -60244,7 +60244,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I2" s="1">
         <v>43228</v>
@@ -60323,7 +60323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -60343,7 +60343,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I3" s="1">
         <v>43228</v>
@@ -60415,14 +60415,14 @@
         <v>0</v>
       </c>
       <c r="AG3" s="19">
-        <f t="shared" ref="AG3:AG66" si="0">+SUM(Y3:AF3)</f>
+        <f t="shared" ref="AG3:AG13" si="0">+SUM(Y3:AF3)</f>
         <v>0</v>
       </c>
       <c r="AI3" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -60442,7 +60442,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I4" s="1">
         <v>45246</v>
@@ -60521,7 +60521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -60541,7 +60541,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I5" s="1">
         <v>45246</v>
@@ -60620,7 +60620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -60640,7 +60640,7 @@
         <v>8</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I6" s="1">
         <v>45246</v>
@@ -60719,7 +60719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -60739,7 +60739,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I7" s="1">
         <v>45246</v>
@@ -60818,7 +60818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -60838,7 +60838,7 @@
         <v>124</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I8" s="1">
         <v>55318</v>
@@ -60862,7 +60862,7 @@
         <v>-1</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q8" s="9">
         <v>10</v>
@@ -60917,7 +60917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -60937,7 +60937,7 @@
         <v>64</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I9" s="1">
         <v>53207</v>
@@ -60961,7 +60961,7 @@
         <v>-1</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q9" s="9">
         <v>1</v>
@@ -61010,7 +61010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -61030,7 +61030,7 @@
         <v>64</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I10" s="1">
         <v>53221</v>
@@ -61054,7 +61054,7 @@
         <v>-1</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q10" s="9">
         <v>1</v>
@@ -61103,7 +61103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -61123,7 +61123,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I11" s="1">
         <v>60803</v>
@@ -61202,7 +61202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -61222,7 +61222,7 @@
         <v>23</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I12" s="1">
         <v>41042</v>
@@ -61295,7 +61295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -61315,7 +61315,7 @@
         <v>23</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I13" s="1">
         <v>41042</v>
@@ -61388,7 +61388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -61402,7 +61402,7 @@
         <v>4</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>180</v>
@@ -61423,7 +61423,7 @@
         <v>-1</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Q14" s="9">
         <v>1</v>
@@ -61466,17 +61466,17 @@
         <v>0</v>
       </c>
       <c r="AG14" s="19">
-        <f>+SUM(Y14:AF14)</f>
+        <f t="shared" ref="AG14:AG45" si="1">+SUM(Y14:AF14)</f>
         <v>71500000</v>
       </c>
       <c r="AH14" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI14" s="19">
         <v>163743000</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -61496,7 +61496,7 @@
         <v>54</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I15" s="1">
         <v>75214</v>
@@ -61520,7 +61520,7 @@
         <v>-1</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q15" s="9">
         <v>1</v>
@@ -61568,17 +61568,17 @@
         <v>0</v>
       </c>
       <c r="AG15" s="19">
-        <f>+SUM(Y15:AF15)</f>
+        <f t="shared" si="1"/>
         <v>32779330.879999999</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AI15" s="19">
         <v>37800000</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -61598,7 +61598,7 @@
         <v>83</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I16" s="1">
         <v>75234</v>
@@ -61622,7 +61622,7 @@
         <v>-1</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Q16" s="9">
         <v>1</v>
@@ -61631,7 +61631,7 @@
         <v>42915</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T16" s="1">
         <v>32.902931000000002</v>
@@ -61673,17 +61673,17 @@
         <v>0</v>
       </c>
       <c r="AG16" s="19">
-        <f>+SUM(Y16:AF16)</f>
+        <f t="shared" si="1"/>
         <v>32400000</v>
       </c>
       <c r="AH16" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AI16" s="19">
         <v>55200000</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -61697,13 +61697,13 @@
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I17" s="1">
         <v>75013</v>
@@ -61727,7 +61727,7 @@
         <v>-1</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q17" s="9">
         <v>1</v>
@@ -61736,7 +61736,7 @@
         <v>43348</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="T17" s="1">
         <v>33.118155999999999</v>
@@ -61778,17 +61778,17 @@
         <v>0</v>
       </c>
       <c r="AG17" s="19">
-        <f>+SUM(Y17:AF17)</f>
+        <f t="shared" si="1"/>
         <v>29200000</v>
       </c>
       <c r="AH17" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AI17" s="19">
         <v>47000000</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -61808,7 +61808,7 @@
         <v>181</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I18" s="1">
         <v>87121</v>
@@ -61832,7 +61832,7 @@
         <v>-1</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q18" s="9">
         <v>1</v>
@@ -61880,17 +61880,17 @@
         <v>15769000</v>
       </c>
       <c r="AG18" s="19">
-        <f>+SUM(Y18:AF18)</f>
+        <f t="shared" si="1"/>
         <v>26194000</v>
       </c>
       <c r="AH18" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI18" s="19">
         <v>43575000</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -61910,7 +61910,7 @@
         <v>98</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I19" s="1">
         <v>85281</v>
@@ -61934,7 +61934,7 @@
         <v>-1</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Q19" s="9">
         <v>6</v>
@@ -61982,17 +61982,17 @@
         <v>0</v>
       </c>
       <c r="AG19" s="19">
-        <f>+SUM(Y19:AF19)</f>
+        <f t="shared" si="1"/>
         <v>25750000</v>
       </c>
       <c r="AH19" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI19" s="19">
         <v>33329000</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -62000,19 +62000,19 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I20" s="1">
         <v>75126</v>
@@ -62036,7 +62036,7 @@
         <v>-1</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Q20" s="9">
         <v>1</v>
@@ -62045,7 +62045,7 @@
         <v>43908</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="T20" s="1">
         <v>32.750933000000003</v>
@@ -62087,11 +62087,11 @@
         <v>23058734</v>
       </c>
       <c r="AG20" s="19">
-        <f>+SUM(Y20:AF20)</f>
+        <f t="shared" si="1"/>
         <v>23058734</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -62105,7 +62105,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>174</v>
@@ -62126,7 +62126,7 @@
         <v>12</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q21" s="9">
         <v>10</v>
@@ -62168,17 +62168,17 @@
         <v>0</v>
       </c>
       <c r="AG21" s="19">
-        <f>+SUM(Y21:AF21)</f>
+        <f t="shared" si="1"/>
         <v>20700000</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AI21" s="19">
         <v>38998100</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -62198,7 +62198,7 @@
         <v>139</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I22" s="1">
         <v>55425</v>
@@ -62222,7 +62222,7 @@
         <v>-1</v>
       </c>
       <c r="P22" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q22" s="9">
         <v>9</v>
@@ -62270,14 +62270,14 @@
         <v>0</v>
       </c>
       <c r="AG22" s="19">
-        <f>+SUM(Y22:AF22)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI22" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -62297,7 +62297,7 @@
         <v>118</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I23" s="1">
         <v>55423</v>
@@ -62321,7 +62321,7 @@
         <v>-1</v>
       </c>
       <c r="P23" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q23" s="9">
         <v>8</v>
@@ -62369,14 +62369,14 @@
         <v>0</v>
       </c>
       <c r="AG23" s="19">
-        <f>+SUM(Y23:AF23)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI23" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -62396,7 +62396,7 @@
         <v>146</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I24" s="1">
         <v>55441</v>
@@ -62420,7 +62420,7 @@
         <v>-1</v>
       </c>
       <c r="P24" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q24" s="9">
         <v>5</v>
@@ -62468,14 +62468,14 @@
         <v>0</v>
       </c>
       <c r="AG24" s="19">
-        <f>+SUM(Y24:AF24)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI24" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -62495,7 +62495,7 @@
         <v>179</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I25" s="1">
         <v>77389</v>
@@ -62519,7 +62519,7 @@
         <v>-1</v>
       </c>
       <c r="P25" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q25" s="9">
         <v>1</v>
@@ -62528,7 +62528,7 @@
         <v>43922</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T25" s="1">
         <v>30.091379</v>
@@ -62570,14 +62570,14 @@
         <v>15055000</v>
       </c>
       <c r="AG25" s="19">
-        <f>+SUM(Y25:AF25)</f>
+        <f t="shared" si="1"/>
         <v>20465000</v>
       </c>
       <c r="AI25" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -62597,7 +62597,7 @@
         <v>86</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I26" s="1">
         <v>15212</v>
@@ -62621,7 +62621,7 @@
         <v>-1</v>
       </c>
       <c r="P26" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q26" s="9">
         <v>11</v>
@@ -62669,17 +62669,17 @@
         <v>0</v>
       </c>
       <c r="AG26" s="19">
-        <f>+SUM(Y26:AF26)</f>
+        <f t="shared" si="1"/>
         <v>20100000</v>
       </c>
       <c r="AH26" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI26" s="19">
         <v>40500000</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -62699,7 +62699,7 @@
         <v>89</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I27" s="1">
         <v>32606</v>
@@ -62723,7 +62723,7 @@
         <v>-1</v>
       </c>
       <c r="P27" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q27" s="9">
         <v>1</v>
@@ -62732,7 +62732,7 @@
         <v>43763</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="T27" s="1">
         <v>29.68797</v>
@@ -62774,17 +62774,17 @@
         <v>0</v>
       </c>
       <c r="AG27" s="19">
-        <f>+SUM(Y27:AF27)</f>
+        <f t="shared" si="1"/>
         <v>19700000</v>
       </c>
       <c r="AH27" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AI27" s="19">
         <v>40000000</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -62804,7 +62804,7 @@
         <v>102</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I28" s="1">
         <v>33763</v>
@@ -62828,7 +62828,7 @@
         <v>-1</v>
       </c>
       <c r="P28" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q28" s="9">
         <v>1</v>
@@ -62837,7 +62837,7 @@
         <v>43640</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="T28" s="1">
         <v>28.001814</v>
@@ -62879,17 +62879,17 @@
         <v>0</v>
       </c>
       <c r="AG28" s="19">
-        <f>+SUM(Y28:AF28)</f>
+        <f t="shared" si="1"/>
         <v>18200000</v>
       </c>
       <c r="AH28" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AI28" s="19">
         <v>28312000</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -62909,7 +62909,7 @@
         <v>50</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I29" s="1">
         <v>85014</v>
@@ -62933,7 +62933,7 @@
         <v>-1</v>
       </c>
       <c r="P29" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q29" s="9">
         <v>4</v>
@@ -62981,17 +62981,17 @@
         <v>0</v>
       </c>
       <c r="AG29" s="19">
-        <f>+SUM(Y29:AF29)</f>
+        <f t="shared" si="1"/>
         <v>17250000</v>
       </c>
       <c r="AH29" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI29" s="19">
         <v>19975000</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -63011,7 +63011,7 @@
         <v>8</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I30" s="1">
         <v>45246</v>
@@ -63083,14 +63083,14 @@
         <v>0</v>
       </c>
       <c r="AG30" s="19">
-        <f>+SUM(Y30:AF30)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI30" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -63098,7 +63098,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
@@ -63107,10 +63107,10 @@
         <v>41</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K31" s="1">
         <v>1</v>
@@ -63128,7 +63128,7 @@
         <v>5</v>
       </c>
       <c r="P31" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q31" s="9">
         <v>10</v>
@@ -63170,17 +63170,17 @@
         <v>0</v>
       </c>
       <c r="AG31" s="19">
-        <f>+SUM(Y31:AF31)</f>
+        <f t="shared" si="1"/>
         <v>16140000</v>
       </c>
       <c r="AH31" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AI31" s="19">
         <v>25879374.989999998</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -63200,7 +63200,7 @@
         <v>37</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I32" s="1">
         <v>50266</v>
@@ -63224,7 +63224,7 @@
         <v>-1</v>
       </c>
       <c r="P32" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Q32" s="9">
         <v>7</v>
@@ -63272,17 +63272,17 @@
         <v>0</v>
       </c>
       <c r="AG32" s="19">
-        <f>+SUM(Y32:AF32)</f>
+        <f t="shared" si="1"/>
         <v>15488628</v>
       </c>
       <c r="AH32" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI32" s="19">
         <v>28175000</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -63302,7 +63302,7 @@
         <v>67</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I33" s="1">
         <v>75126</v>
@@ -63326,7 +63326,7 @@
         <v>-1</v>
       </c>
       <c r="P33" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q33" s="9">
         <v>1</v>
@@ -63335,7 +63335,7 @@
         <v>43006</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="T33" s="1">
         <v>32.753647999999998</v>
@@ -63377,17 +63377,17 @@
         <v>3555000</v>
       </c>
       <c r="AG33" s="19">
-        <f>+SUM(Y33:AF33)</f>
+        <f t="shared" si="1"/>
         <v>15000000</v>
       </c>
       <c r="AH33" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AI33" s="19">
         <v>25350000</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -63395,7 +63395,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E34" s="1">
         <v>5</v>
@@ -63407,7 +63407,7 @@
         <v>107</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I34" s="1">
         <v>53188</v>
@@ -63431,7 +63431,7 @@
         <v>-1</v>
       </c>
       <c r="P34" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Q34" s="9">
         <v>1</v>
@@ -63440,7 +63440,7 @@
         <v>42765</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T34" s="1">
         <v>43.000940999999997</v>
@@ -63482,11 +63482,11 @@
         <v>0</v>
       </c>
       <c r="AG34" s="19">
-        <f>+SUM(Y34:AF34)</f>
+        <f t="shared" si="1"/>
         <v>14650000</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -63506,7 +63506,7 @@
         <v>127</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I35" s="1">
         <v>55337</v>
@@ -63530,7 +63530,7 @@
         <v>-1</v>
       </c>
       <c r="P35" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q35" s="9">
         <v>10</v>
@@ -63578,14 +63578,14 @@
         <v>0</v>
       </c>
       <c r="AG35" s="19">
-        <f>+SUM(Y35:AF35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI35" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -63605,7 +63605,7 @@
         <v>3</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I36" s="1">
         <v>43217</v>
@@ -63677,14 +63677,14 @@
         <v>0</v>
       </c>
       <c r="AG36" s="19">
-        <f>+SUM(Y36:AF36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI36" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -63704,7 +63704,7 @@
         <v>76</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I37" s="1">
         <v>75051</v>
@@ -63728,7 +63728,7 @@
         <v>-1</v>
       </c>
       <c r="P37" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q37" s="9">
         <v>1</v>
@@ -63737,7 +63737,7 @@
         <v>43221</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="T37" s="1">
         <v>32.733854000000001</v>
@@ -63779,17 +63779,17 @@
         <v>0</v>
       </c>
       <c r="AG37" s="19">
-        <f>+SUM(Y37:AF37)</f>
+        <f t="shared" si="1"/>
         <v>14600000</v>
       </c>
       <c r="AH37" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI37" s="19">
         <v>18995000</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -63809,7 +63809,7 @@
         <v>59</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I38" s="1">
         <v>77505</v>
@@ -63833,7 +63833,7 @@
         <v>-1</v>
       </c>
       <c r="P38" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q38" s="9">
         <v>1</v>
@@ -63842,7 +63842,7 @@
         <v>43417</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="T38" s="1">
         <v>29.638172999999998</v>
@@ -63884,17 +63884,17 @@
         <v>0</v>
       </c>
       <c r="AG38" s="19">
-        <f>+SUM(Y38:AF38)</f>
+        <f t="shared" si="1"/>
         <v>14150000</v>
       </c>
       <c r="AH38" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI38" s="19">
         <v>23120000</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -63914,7 +63914,7 @@
         <v>54</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I39" s="1">
         <v>75252</v>
@@ -63938,7 +63938,7 @@
         <v>-1</v>
       </c>
       <c r="P39" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q39" s="9">
         <v>1</v>
@@ -63947,7 +63947,7 @@
         <v>42491</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T39" s="1">
         <v>32.989317</v>
@@ -63989,17 +63989,17 @@
         <v>0</v>
       </c>
       <c r="AG39" s="19">
-        <f>+SUM(Y39:AF39)</f>
+        <f t="shared" si="1"/>
         <v>13500000</v>
       </c>
       <c r="AH39" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AI39" s="19">
         <v>27580524.309999999</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -64019,7 +64019,7 @@
         <v>79</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I40" s="1">
         <v>64083</v>
@@ -64043,7 +64043,7 @@
         <v>-1</v>
       </c>
       <c r="P40" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q40" s="9">
         <v>6</v>
@@ -64091,17 +64091,17 @@
         <v>0</v>
       </c>
       <c r="AG40" s="19">
-        <f>+SUM(Y40:AF40)</f>
+        <f t="shared" si="1"/>
         <v>13360000</v>
       </c>
       <c r="AH40" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI40" s="19">
         <v>24518000</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -64121,7 +64121,7 @@
         <v>43</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I41" s="1">
         <v>19468</v>
@@ -64145,7 +64145,7 @@
         <v>-1</v>
       </c>
       <c r="P41" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q41" s="9">
         <v>3</v>
@@ -64193,17 +64193,17 @@
         <v>0</v>
       </c>
       <c r="AG41" s="19">
-        <f>+SUM(Y41:AF41)</f>
+        <f t="shared" si="1"/>
         <v>13098000</v>
       </c>
       <c r="AH41" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI41" s="19">
         <v>29002000</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -64223,7 +64223,7 @@
         <v>92</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I42" s="1">
         <v>30047</v>
@@ -64247,7 +64247,7 @@
         <v>-1</v>
       </c>
       <c r="P42" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q42" s="9">
         <v>2</v>
@@ -64295,17 +64295,17 @@
         <v>0</v>
       </c>
       <c r="AG42" s="19">
-        <f>+SUM(Y42:AF42)</f>
+        <f t="shared" si="1"/>
         <v>12796000</v>
       </c>
       <c r="AH42" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AI42" s="19">
         <v>21657000</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -64325,7 +64325,7 @@
         <v>57</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I43" s="1">
         <v>76132</v>
@@ -64349,7 +64349,7 @@
         <v>-1</v>
       </c>
       <c r="P43" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q43" s="9">
         <v>1</v>
@@ -64358,7 +64358,7 @@
         <v>43529</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T43" s="1">
         <v>32.989317</v>
@@ -64400,17 +64400,17 @@
         <v>0</v>
       </c>
       <c r="AG43" s="19">
-        <f>+SUM(Y43:AF43)</f>
+        <f t="shared" si="1"/>
         <v>12550000</v>
       </c>
       <c r="AH43" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI43" s="19">
         <v>17387000</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -64430,7 +64430,7 @@
         <v>47</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I44" s="1">
         <v>33610</v>
@@ -64454,7 +64454,7 @@
         <v>15</v>
       </c>
       <c r="P44" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q44" s="9">
         <v>1</v>
@@ -64502,17 +64502,17 @@
         <v>0</v>
       </c>
       <c r="AG44" s="19">
-        <f>+SUM(Y44:AF44)</f>
+        <f t="shared" si="1"/>
         <v>11900000</v>
       </c>
       <c r="AH44" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AI44" s="19">
         <v>21300000</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -64532,7 +64532,7 @@
         <v>70</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I45" s="1">
         <v>30087</v>
@@ -64556,7 +64556,7 @@
         <v>-1</v>
       </c>
       <c r="P45" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Q45" s="9">
         <v>3</v>
@@ -64604,17 +64604,17 @@
         <v>0</v>
       </c>
       <c r="AG45" s="19">
-        <f>+SUM(Y45:AF45)</f>
+        <f t="shared" si="1"/>
         <v>11050000</v>
       </c>
       <c r="AH45" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AI45" s="19">
         <v>24950000</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -64622,19 +64622,19 @@
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H46" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I46" s="1">
         <v>53213</v>
@@ -64658,7 +64658,7 @@
         <v>-1</v>
       </c>
       <c r="P46" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Q46" s="13">
         <v>1</v>
@@ -64667,7 +64667,7 @@
         <v>43556</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="T46" s="1">
         <v>43.041727999999999</v>
@@ -64709,11 +64709,11 @@
         <v>10000000</v>
       </c>
       <c r="AG46" s="19">
-        <f>+SUM(Y46:AF46)</f>
+        <f t="shared" ref="AG46:AG77" si="2">+SUM(Y46:AF46)</f>
         <v>10000000</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -64733,7 +64733,7 @@
         <v>146</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I47" s="1">
         <v>55441</v>
@@ -64757,7 +64757,7 @@
         <v>-1</v>
       </c>
       <c r="P47" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q47" s="9">
         <v>5</v>
@@ -64805,14 +64805,14 @@
         <v>0</v>
       </c>
       <c r="AG47" s="19">
-        <f>+SUM(Y47:AF47)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI47" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -64820,19 +64820,19 @@
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I48" s="1">
         <v>53402</v>
@@ -64856,7 +64856,7 @@
         <v>-1</v>
       </c>
       <c r="P48" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q48" s="13">
         <v>1</v>
@@ -64865,7 +64865,7 @@
         <v>43874</v>
       </c>
       <c r="S48" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="T48" s="1">
         <v>42.765991</v>
@@ -64907,11 +64907,11 @@
         <v>8179995.3200000003</v>
       </c>
       <c r="AG48" s="19">
-        <f>+SUM(Y48:AF48)</f>
+        <f t="shared" si="2"/>
         <v>8179995.3200000003</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -64928,7 +64928,7 @@
         <v>41</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>41</v>
@@ -64949,7 +64949,7 @@
         <v>7</v>
       </c>
       <c r="P49" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q49" s="9">
         <v>8</v>
@@ -64991,17 +64991,17 @@
         <v>0</v>
       </c>
       <c r="AG49" s="19">
-        <f>+SUM(Y49:AF49)</f>
+        <f t="shared" si="2"/>
         <v>7720000</v>
       </c>
       <c r="AH49" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AI49" s="19">
         <v>7578250</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -65009,16 +65009,16 @@
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H50" s="17">
         <v>55</v>
@@ -65054,7 +65054,7 @@
         <v>43556</v>
       </c>
       <c r="S50" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="T50" s="1">
         <v>42.988776000000001</v>
@@ -65096,14 +65096,14 @@
         <v>7500000</v>
       </c>
       <c r="AG50" s="19">
-        <f>+SUM(Y50:AF50)</f>
+        <f t="shared" si="2"/>
         <v>7500000</v>
       </c>
       <c r="AI50" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -65123,7 +65123,7 @@
         <v>130</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I51" s="1">
         <v>55344</v>
@@ -65147,7 +65147,7 @@
         <v>-1</v>
       </c>
       <c r="P51" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q51" s="9">
         <v>10</v>
@@ -65195,14 +65195,14 @@
         <v>0</v>
       </c>
       <c r="AG51" s="19">
-        <f>+SUM(Y51:AF51)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI51" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -65219,7 +65219,7 @@
         <v>41</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>41</v>
@@ -65240,7 +65240,7 @@
         <v>3</v>
       </c>
       <c r="P52" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q52" s="9">
         <v>9</v>
@@ -65282,17 +65282,17 @@
         <v>0</v>
       </c>
       <c r="AG52" s="19">
-        <f>+SUM(Y52:AF52)</f>
+        <f t="shared" si="2"/>
         <v>6555945.9800000004</v>
       </c>
       <c r="AH52" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AI52" s="19">
         <v>5094679</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -65312,7 +65312,7 @@
         <v>130</v>
       </c>
       <c r="H53" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I53" s="1">
         <v>55344</v>
@@ -65336,7 +65336,7 @@
         <v>-1</v>
       </c>
       <c r="P53" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q53" s="9">
         <v>10</v>
@@ -65384,14 +65384,14 @@
         <v>0</v>
       </c>
       <c r="AG53" s="19">
-        <f>+SUM(Y53:AF53)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI53" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -65411,7 +65411,7 @@
         <v>63</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I54" s="1">
         <v>53233</v>
@@ -65435,7 +65435,7 @@
         <v>-1</v>
       </c>
       <c r="P54" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q54" s="9">
         <v>1</v>
@@ -65444,7 +65444,7 @@
         <v>43545</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="T54" s="1">
         <v>43.045977000000001</v>
@@ -65486,17 +65486,17 @@
         <v>0</v>
       </c>
       <c r="AG54" s="19">
-        <f>+SUM(Y54:AF54)</f>
+        <f t="shared" si="2"/>
         <v>6087942</v>
       </c>
       <c r="AH54" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AI54" s="19">
         <v>6250000</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -65513,7 +65513,7 @@
         <v>64</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>64</v>
@@ -65534,7 +65534,7 @@
         <v>3</v>
       </c>
       <c r="P55" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q55" s="9">
         <v>1</v>
@@ -65582,17 +65582,17 @@
         <v>0</v>
       </c>
       <c r="AG55" s="19">
-        <f>+SUM(Y55:AF55)</f>
+        <f t="shared" si="2"/>
         <v>4720000</v>
       </c>
       <c r="AH55" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AI55" s="19">
         <v>3709430</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -65609,7 +65609,7 @@
         <v>41</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>41</v>
@@ -65630,7 +65630,7 @@
         <v>7</v>
       </c>
       <c r="P56" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q56" s="9">
         <v>5</v>
@@ -65678,17 +65678,17 @@
         <v>0</v>
       </c>
       <c r="AG56" s="19">
-        <f>+SUM(Y56:AF56)</f>
+        <f t="shared" si="2"/>
         <v>3950000</v>
       </c>
       <c r="AH56" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AI56" s="19">
         <v>6115285</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -65696,7 +65696,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>165</v>
@@ -65711,7 +65711,7 @@
         <v>60</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I57" s="1">
         <v>77090</v>
@@ -65735,7 +65735,7 @@
         <v>-1</v>
       </c>
       <c r="P57" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q57" s="9">
         <v>1</v>
@@ -65744,7 +65744,7 @@
         <v>43817</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T57" s="1">
         <v>30.027327</v>
@@ -65786,17 +65786,17 @@
         <v>0</v>
       </c>
       <c r="AG57" s="19">
-        <f>+SUM(Y57:AF57)</f>
+        <f t="shared" si="2"/>
         <v>9705882.3529411759</v>
       </c>
       <c r="AH57" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI57" s="19">
         <v>24336000</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -65804,7 +65804,7 @@
         <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>163</v>
@@ -65819,7 +65819,7 @@
         <v>60</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I58" s="1">
         <v>77066</v>
@@ -65843,7 +65843,7 @@
         <v>-1</v>
       </c>
       <c r="P58" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q58" s="9">
         <v>1</v>
@@ -65852,7 +65852,7 @@
         <v>43817</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="T58" s="1">
         <v>29.981292</v>
@@ -65894,17 +65894,17 @@
         <v>0</v>
       </c>
       <c r="AG58" s="19">
-        <f>+SUM(Y58:AF58)</f>
+        <f t="shared" si="2"/>
         <v>7683823.5294117648</v>
       </c>
       <c r="AH58" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI58" s="19">
         <v>18000000</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -65912,7 +65912,7 @@
         <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>157</v>
@@ -65927,7 +65927,7 @@
         <v>154</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I59" s="1">
         <v>74136</v>
@@ -65951,7 +65951,7 @@
         <v>-1</v>
       </c>
       <c r="P59" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q59" s="9">
         <v>1</v>
@@ -65960,7 +65960,7 @@
         <v>43817</v>
       </c>
       <c r="S59" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="T59" s="1">
         <v>36.065963000000004</v>
@@ -66002,17 +66002,17 @@
         <v>0</v>
       </c>
       <c r="AG59" s="19">
-        <f>+SUM(Y59:AF59)</f>
+        <f t="shared" si="2"/>
         <v>2992647.0588235292</v>
       </c>
       <c r="AH59" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI59" s="19">
         <v>6162000</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -66020,7 +66020,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>149</v>
@@ -66035,7 +66035,7 @@
         <v>151</v>
       </c>
       <c r="H60" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I60" s="1">
         <v>73120</v>
@@ -66059,7 +66059,7 @@
         <v>-1</v>
       </c>
       <c r="P60" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q60" s="9">
         <v>1</v>
@@ -66068,7 +66068,7 @@
         <v>43817</v>
       </c>
       <c r="S60" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T60" s="1">
         <v>35.597188000000003</v>
@@ -66110,17 +66110,17 @@
         <v>0</v>
       </c>
       <c r="AG60" s="19">
-        <f>+SUM(Y60:AF60)</f>
+        <f t="shared" si="2"/>
         <v>10838235.294117648</v>
       </c>
       <c r="AH60" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI60" s="19">
         <v>24535000</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -66128,7 +66128,7 @@
         <v>0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>152</v>
@@ -66143,7 +66143,7 @@
         <v>154</v>
       </c>
       <c r="H61" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I61" s="1">
         <v>74132</v>
@@ -66167,7 +66167,7 @@
         <v>-1</v>
       </c>
       <c r="P61" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q61" s="9">
         <v>1</v>
@@ -66176,7 +66176,7 @@
         <v>43817</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="T61" s="1">
         <v>36.071460999999999</v>
@@ -66218,17 +66218,17 @@
         <v>0</v>
       </c>
       <c r="AG61" s="19">
-        <f>+SUM(Y61:AF61)</f>
+        <f t="shared" si="2"/>
         <v>5985294.1176470583</v>
       </c>
       <c r="AH61" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI61" s="19">
         <v>13486000</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -66236,7 +66236,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>155</v>
@@ -66251,7 +66251,7 @@
         <v>151</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I62" s="1">
         <v>73114</v>
@@ -66275,7 +66275,7 @@
         <v>-1</v>
       </c>
       <c r="P62" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q62" s="9">
         <v>1</v>
@@ -66284,7 +66284,7 @@
         <v>43817</v>
       </c>
       <c r="S62" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T62" s="1">
         <v>35.581014000000003</v>
@@ -66326,17 +66326,17 @@
         <v>0</v>
       </c>
       <c r="AG62" s="19">
-        <f>+SUM(Y62:AF62)</f>
+        <f t="shared" si="2"/>
         <v>3720588.2352941176</v>
       </c>
       <c r="AH62" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI62" s="19">
         <v>8408000</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -66344,7 +66344,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>167</v>
@@ -66359,7 +66359,7 @@
         <v>60</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I63" s="1">
         <v>77079</v>
@@ -66383,7 +66383,7 @@
         <v>-1</v>
       </c>
       <c r="P63" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q63" s="9">
         <v>1</v>
@@ -66392,7 +66392,7 @@
         <v>43817</v>
       </c>
       <c r="S63" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="T63" s="1">
         <v>29.777594000000001</v>
@@ -66434,17 +66434,17 @@
         <v>0</v>
       </c>
       <c r="AG63" s="19">
-        <f>+SUM(Y63:AF63)</f>
+        <f t="shared" si="2"/>
         <v>4852941.176470588</v>
       </c>
       <c r="AH63" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI63" s="19">
         <v>11330000</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -66452,7 +66452,7 @@
         <v>0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>159</v>
@@ -66467,7 +66467,7 @@
         <v>151</v>
       </c>
       <c r="H64" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I64" s="1">
         <v>73142</v>
@@ -66491,7 +66491,7 @@
         <v>-1</v>
       </c>
       <c r="P64" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q64" s="9">
         <v>1</v>
@@ -66500,7 +66500,7 @@
         <v>43817</v>
       </c>
       <c r="S64" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T64" s="1">
         <v>35.595573000000002</v>
@@ -66542,17 +66542,17 @@
         <v>0</v>
       </c>
       <c r="AG64" s="19">
-        <f>+SUM(Y64:AF64)</f>
+        <f t="shared" si="2"/>
         <v>2102941.1764705884</v>
       </c>
       <c r="AH64" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI64" s="19">
         <v>4859000</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
@@ -66560,7 +66560,7 @@
         <v>0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>161</v>
@@ -66575,7 +66575,7 @@
         <v>60</v>
       </c>
       <c r="H65" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I65" s="1">
         <v>77077</v>
@@ -66599,7 +66599,7 @@
         <v>-1</v>
       </c>
       <c r="P65" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q65" s="9">
         <v>1</v>
@@ -66608,7 +66608,7 @@
         <v>43817</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T65" s="1">
         <v>29.738977999999999</v>
@@ -66650,17 +66650,17 @@
         <v>0</v>
       </c>
       <c r="AG65" s="19">
-        <f>+SUM(Y65:AF65)</f>
+        <f t="shared" si="2"/>
         <v>10352941.176470589</v>
       </c>
       <c r="AH65" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI65" s="19">
         <v>22470000</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -66680,7 +66680,7 @@
         <v>121</v>
       </c>
       <c r="H66" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I66" s="1">
         <v>55369</v>
@@ -66704,7 +66704,7 @@
         <v>-1</v>
       </c>
       <c r="P66" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q66" s="9">
         <v>8</v>
@@ -66752,14 +66752,14 @@
         <v>0</v>
       </c>
       <c r="AG66" s="19">
-        <f>+SUM(Y66:AF66)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI66" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -66779,7 +66779,7 @@
         <v>40</v>
       </c>
       <c r="H67" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I67" s="1">
         <v>55427</v>
@@ -66803,7 +66803,7 @@
         <v>1</v>
       </c>
       <c r="P67" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q67" s="9">
         <v>12</v>
@@ -66845,17 +66845,17 @@
         <v>0</v>
       </c>
       <c r="AG67" s="19">
-        <f>+SUM(Y67:AF67)</f>
+        <f t="shared" si="2"/>
         <v>3683000</v>
       </c>
       <c r="AH67" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AI67" s="19">
         <v>5309009</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>0</v>
       </c>
@@ -66878,7 +66878,7 @@
         <v>151</v>
       </c>
       <c r="H68" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I68" s="1">
         <v>73112</v>
@@ -66902,7 +66902,7 @@
         <v>-1</v>
       </c>
       <c r="P68" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q68" s="9">
         <v>1</v>
@@ -66911,7 +66911,7 @@
         <v>43817</v>
       </c>
       <c r="S68" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T68" s="1">
         <v>35.527355</v>
@@ -66953,17 +66953,17 @@
         <v>0</v>
       </c>
       <c r="AG68" s="19">
-        <f>+SUM(Y68:AF68)</f>
+        <f t="shared" si="2"/>
         <v>13264705.882352943</v>
       </c>
       <c r="AH68" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AI68" s="19">
         <v>30157000</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -66983,7 +66983,7 @@
         <v>139</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I69" s="1">
         <v>55431</v>
@@ -67007,7 +67007,7 @@
         <v>1</v>
       </c>
       <c r="P69" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Q69" s="9">
         <v>9</v>
@@ -67055,17 +67055,17 @@
         <v>0</v>
       </c>
       <c r="AG69" s="19">
-        <f>+SUM(Y69:AF69)</f>
+        <f t="shared" si="2"/>
         <v>3250000</v>
       </c>
       <c r="AH69" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI69" s="19">
         <v>3900000</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
@@ -67073,19 +67073,19 @@
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E70" s="1">
         <v>1</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>107</v>
       </c>
       <c r="H70" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I70" s="1">
         <v>53186</v>
@@ -67109,7 +67109,7 @@
         <v>-1</v>
       </c>
       <c r="P70" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q70" s="13">
         <v>1</v>
@@ -67118,7 +67118,7 @@
         <v>43908</v>
       </c>
       <c r="S70" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="T70" s="1">
         <v>43.012256999999998</v>
@@ -67160,11 +67160,11 @@
         <v>3056134.61</v>
       </c>
       <c r="AG70" s="19">
-        <f>+SUM(Y70:AF70)</f>
+        <f t="shared" si="2"/>
         <v>3056134.61</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
@@ -67172,25 +67172,25 @@
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E71" s="1">
         <v>1</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H71" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I71" s="1">
         <v>76051</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K71" s="1">
         <v>2</v>
@@ -67217,7 +67217,7 @@
         <v>36972</v>
       </c>
       <c r="S71" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="T71" s="1">
         <v>32.957152000000001</v>
@@ -67259,11 +67259,11 @@
         <v>0</v>
       </c>
       <c r="AG71" s="19">
-        <f>+SUM(Y71:AF71)</f>
+        <f t="shared" si="2"/>
         <v>2850000</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -67283,7 +67283,7 @@
         <v>135</v>
       </c>
       <c r="H72" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I72" s="1">
         <v>55379</v>
@@ -67307,7 +67307,7 @@
         <v>-1</v>
       </c>
       <c r="P72" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q72" s="9">
         <v>10</v>
@@ -67355,14 +67355,14 @@
         <v>0</v>
       </c>
       <c r="AG72" s="19">
-        <f>+SUM(Y72:AF72)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI72" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -67382,7 +67382,7 @@
         <v>139</v>
       </c>
       <c r="H73" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I73" s="1">
         <v>55437</v>
@@ -67406,7 +67406,7 @@
         <v>-1</v>
       </c>
       <c r="P73" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q73" s="9">
         <v>9</v>
@@ -67454,14 +67454,14 @@
         <v>0</v>
       </c>
       <c r="AG73" s="19">
-        <f>+SUM(Y73:AF73)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI73" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
@@ -67481,7 +67481,7 @@
         <v>64</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I74" s="1">
         <v>53207</v>
@@ -67505,7 +67505,7 @@
         <v>-1</v>
       </c>
       <c r="P74" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q74" s="9">
         <v>1</v>
@@ -67553,14 +67553,14 @@
         <v>0</v>
       </c>
       <c r="AG74" s="19">
-        <f>+SUM(Y74:AF74)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI74" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -67580,7 +67580,7 @@
         <v>41</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I75" s="1">
         <v>55404</v>
@@ -67604,7 +67604,7 @@
         <v>1</v>
       </c>
       <c r="P75" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Q75" s="9">
         <v>8</v>
@@ -67646,14 +67646,14 @@
         <v>0</v>
       </c>
       <c r="AG75" s="19">
-        <f>+SUM(Y75:AF75)</f>
+        <f t="shared" si="2"/>
         <v>2500000</v>
       </c>
       <c r="AI75" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
@@ -67673,7 +67673,7 @@
         <v>3</v>
       </c>
       <c r="H76" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I76" s="1">
         <v>43228</v>
@@ -67745,14 +67745,14 @@
         <v>0</v>
       </c>
       <c r="AG76" s="19">
-        <f>+SUM(Y76:AF76)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI76" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -67763,7 +67763,7 @@
         <v>186</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E77" s="1">
         <v>5</v>
@@ -67772,10 +67772,10 @@
         <v>55</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I77" s="1">
         <v>55430</v>
@@ -67799,7 +67799,7 @@
         <v>1</v>
       </c>
       <c r="P77" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q77" s="9">
         <v>8</v>
@@ -67847,17 +67847,17 @@
         <v>0</v>
       </c>
       <c r="AG77" s="19">
-        <f>+SUM(Y77:AF77)</f>
+        <f t="shared" si="2"/>
         <v>2418931</v>
       </c>
       <c r="AH77" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AI77" s="19">
         <v>5282430</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -67871,13 +67871,13 @@
         <v>9</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>136</v>
       </c>
       <c r="H78" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I78" s="1">
         <v>53130</v>
@@ -67901,7 +67901,7 @@
         <v>-1</v>
       </c>
       <c r="P78" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q78" s="9">
         <v>1</v>
@@ -67949,11 +67949,11 @@
         <v>0</v>
       </c>
       <c r="AG78" s="19">
-        <f>+SUM(Y78:AF78)</f>
+        <f t="shared" ref="AG78:AG109" si="3">+SUM(Y78:AF78)</f>
         <v>2200001</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -67973,7 +67973,7 @@
         <v>95</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I79" s="1">
         <v>55112</v>
@@ -67997,7 +67997,7 @@
         <v>2</v>
       </c>
       <c r="P79" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q79" s="9">
         <v>5</v>
@@ -68045,17 +68045,17 @@
         <v>0</v>
       </c>
       <c r="AG79" s="19">
-        <f>+SUM(Y79:AF79)</f>
+        <f t="shared" si="3"/>
         <v>2154904</v>
       </c>
       <c r="AH79" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AI79" s="19">
         <v>3487500</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -68075,7 +68075,7 @@
         <v>33</v>
       </c>
       <c r="H80" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I80" s="1">
         <v>60173</v>
@@ -68099,7 +68099,7 @@
         <v>1</v>
       </c>
       <c r="P80" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q80" s="9">
         <v>1</v>
@@ -68147,17 +68147,17 @@
         <v>0</v>
       </c>
       <c r="AG80" s="19">
-        <f>+SUM(Y80:AF80)</f>
+        <f t="shared" si="3"/>
         <v>1900000</v>
       </c>
       <c r="AH80" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI80" s="19">
         <v>2179345</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -68165,22 +68165,22 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H81" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I81" s="1">
         <v>53151</v>
@@ -68204,7 +68204,7 @@
         <v>-1</v>
       </c>
       <c r="P81" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q81" s="13">
         <v>1</v>
@@ -68252,11 +68252,11 @@
         <v>1693242.59</v>
       </c>
       <c r="AG81" s="19">
-        <f>+SUM(Y81:AF81)</f>
+        <f t="shared" si="3"/>
         <v>1693242.59</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
@@ -68276,7 +68276,7 @@
         <v>105</v>
       </c>
       <c r="H82" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I82" s="1">
         <v>53029</v>
@@ -68300,7 +68300,7 @@
         <v>-1</v>
       </c>
       <c r="P82" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q82" s="9">
         <v>1</v>
@@ -68348,14 +68348,14 @@
         <v>0</v>
       </c>
       <c r="AG82" s="19">
-        <f>+SUM(Y82:AF82)</f>
+        <f t="shared" si="3"/>
         <v>870699</v>
       </c>
       <c r="AI82" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
@@ -68363,25 +68363,25 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E83" s="1">
         <v>1</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="G83" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="H83" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I83" s="1">
         <v>75087</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K83" s="1">
         <v>2</v>
@@ -68408,7 +68408,7 @@
         <v>33938</v>
       </c>
       <c r="S83" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="T83" s="1">
         <v>32.913938000000002</v>
@@ -68450,11 +68450,11 @@
         <v>0</v>
       </c>
       <c r="AG83" s="19">
-        <f>+SUM(Y83:AF83)</f>
+        <f t="shared" si="3"/>
         <v>825000</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -68462,25 +68462,25 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E84" s="1">
         <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G84" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="H84" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I84" s="1">
         <v>75043</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K84" s="1">
         <v>2</v>
@@ -68507,7 +68507,7 @@
         <v>33324</v>
       </c>
       <c r="S84" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="T84" s="1">
         <v>32.848539000000002</v>
@@ -68549,28 +68549,28 @@
         <v>0</v>
       </c>
       <c r="AG84" s="19">
-        <f>+SUM(Y84:AF84)</f>
+        <f t="shared" si="3"/>
         <v>731616</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B85" s="16">
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E85" s="1">
         <v>1</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H85" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M85" s="1">
         <v>0</v>
@@ -68579,7 +68579,7 @@
         <v>0</v>
       </c>
       <c r="P85" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R85" s="10">
         <v>41791</v>
@@ -68618,7 +68618,7 @@
         <v>0</v>
       </c>
       <c r="AG85" s="19">
-        <f>+SUM(Y85:AF85)</f>
+        <f t="shared" si="3"/>
         <v>600000</v>
       </c>
     </row>
@@ -68641,7 +68641,7 @@
       <selection sqref="A1:A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added missing db cols
</commit_message>
<xml_diff>
--- a/data/db/properties.xlsx
+++ b/data/db/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nburmeister\Documents\_Development\AssetManagementPortal\data\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0AD85B-F66D-4C7D-8BA2-E4F73A8308E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181B677F-FA64-461A-B1EC-A5750AD3AC74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{65CCAB74-0CA2-4D5F-9FC7-1AACCFC26E43}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{65CCAB74-0CA2-4D5F-9FC7-1AACCFC26E43}"/>
   </bookViews>
   <sheets>
     <sheet name="PropertyData" sheetId="1" r:id="rId1"/>
@@ -4492,9 +4492,6 @@
     <t>mlg_historical_equity</t>
   </si>
   <si>
-    <t>managed_account</t>
-  </si>
-  <si>
     <t>Gateway Pines</t>
   </si>
   <si>
@@ -4616,6 +4613,9 @@
   </si>
   <si>
     <t>property_name</t>
+  </si>
+  <si>
+    <t>managed_account_equity</t>
   </si>
 </sst>
 </file>
@@ -60072,10 +60072,10 @@
   <dimension ref="A1:AI85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60125,7 +60125,7 @@
         <v>191</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>258</v>
@@ -60212,7 +60212,7 @@
         <v>321</v>
       </c>
       <c r="AF1" s="19" t="s">
-        <v>322</v>
+        <v>363</v>
       </c>
       <c r="AG1" s="19" t="s">
         <v>303</v>
@@ -62000,13 +62000,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>67</v>
@@ -62036,7 +62036,7 @@
         <v>-1</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="Q20" s="9">
         <v>1</v>
@@ -62045,7 +62045,7 @@
         <v>43908</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="T20" s="1">
         <v>32.750933000000003</v>
@@ -64622,16 +64622,16 @@
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H46" s="20" t="s">
         <v>218</v>
@@ -64658,7 +64658,7 @@
         <v>-1</v>
       </c>
       <c r="P46" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q46" s="13">
         <v>1</v>
@@ -64667,7 +64667,7 @@
         <v>43556</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="T46" s="1">
         <v>43.041727999999999</v>
@@ -64820,16 +64820,16 @@
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H48" s="20" t="s">
         <v>218</v>
@@ -64856,7 +64856,7 @@
         <v>-1</v>
       </c>
       <c r="P48" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q48" s="13">
         <v>1</v>
@@ -64865,7 +64865,7 @@
         <v>43874</v>
       </c>
       <c r="S48" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="T48" s="1">
         <v>42.765991</v>
@@ -67073,13 +67073,13 @@
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E70" s="1">
         <v>1</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>107</v>
@@ -67109,7 +67109,7 @@
         <v>-1</v>
       </c>
       <c r="P70" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q70" s="13">
         <v>1</v>
@@ -67118,7 +67118,7 @@
         <v>43908</v>
       </c>
       <c r="S70" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="T70" s="1">
         <v>43.012256999999998</v>
@@ -67172,16 +67172,16 @@
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E71" s="1">
         <v>1</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H71" s="20" t="s">
         <v>217</v>
@@ -67190,7 +67190,7 @@
         <v>76051</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K71" s="1">
         <v>2</v>
@@ -67217,7 +67217,7 @@
         <v>36972</v>
       </c>
       <c r="S71" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="T71" s="1">
         <v>32.957152000000001</v>
@@ -67763,7 +67763,7 @@
         <v>186</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E77" s="1">
         <v>5</v>
@@ -67949,7 +67949,7 @@
         <v>0</v>
       </c>
       <c r="AG78" s="19">
-        <f t="shared" ref="AG78:AG109" si="3">+SUM(Y78:AF78)</f>
+        <f t="shared" ref="AG78:AG85" si="3">+SUM(Y78:AF78)</f>
         <v>2200001</v>
       </c>
     </row>
@@ -68049,7 +68049,7 @@
         <v>2154904</v>
       </c>
       <c r="AH79" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AI79" s="19">
         <v>3487500</v>
@@ -68165,16 +68165,16 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>222</v>
@@ -68204,7 +68204,7 @@
         <v>-1</v>
       </c>
       <c r="P81" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q81" s="13">
         <v>1</v>
@@ -68363,16 +68363,16 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E83" s="1">
         <v>1</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>354</v>
       </c>
       <c r="H83" s="20" t="s">
         <v>217</v>
@@ -68381,7 +68381,7 @@
         <v>75087</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K83" s="1">
         <v>2</v>
@@ -68408,7 +68408,7 @@
         <v>33938</v>
       </c>
       <c r="S83" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="T83" s="1">
         <v>32.913938000000002</v>
@@ -68462,16 +68462,16 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E84" s="1">
         <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="H84" s="20" t="s">
         <v>217</v>
@@ -68480,7 +68480,7 @@
         <v>75043</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K84" s="1">
         <v>2</v>
@@ -68507,7 +68507,7 @@
         <v>33324</v>
       </c>
       <c r="S84" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="T84" s="1">
         <v>32.848539000000002</v>
@@ -68555,19 +68555,19 @@
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B85" s="16">
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E85" s="1">
         <v>1</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H85" s="20" t="s">
         <v>218</v>
@@ -68579,7 +68579,7 @@
         <v>0</v>
       </c>
       <c r="P85" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="R85" s="10">
         <v>41791</v>

</xml_diff>